<commit_message>
Revisão parcial dos artefatos da 2a. entrega.
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="390" yWindow="510" windowWidth="20775" windowHeight="9405"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Página1" state="visible" r:id="rId3"/>
+    <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>REQ(01)</t>
   </si>
@@ -91,7 +94,7 @@
     <t>Selecionar Preço</t>
   </si>
   <si>
-    <t> </t>
+    <t/>
   </si>
   <si>
     <t>REQ(09)</t>
@@ -160,37 +163,64 @@
     <t>UC09 - Selecionar Preço</t>
   </si>
   <si>
-    <t>UC10 - Comprar Ingresso</t>
-  </si>
-  <si>
-    <t>UC11 - Cancelar Compra</t>
-  </si>
-  <si>
-    <t>UC12 - Receber Dinheiro</t>
+    <t>Selecionar filmes, salas, sessões, preço, faz parte de um mesmo UC (Comprar Ingresso). Não faz sentido serem UCs separados!</t>
+  </si>
+  <si>
+    <t>UC06 - Comprar Ingresso</t>
+  </si>
+  <si>
+    <t>UC07 - Cancelar Compra</t>
+  </si>
+  <si>
+    <t>Carregar Troco</t>
+  </si>
+  <si>
+    <t>UC09 - Carregar Troco</t>
+  </si>
+  <si>
+    <t>Carga de papel para emissão de ingressos ??</t>
+  </si>
+  <si>
+    <t>Relatórios de vendas ??</t>
+  </si>
+  <si>
+    <t>Receber Pagamento</t>
+  </si>
+  <si>
+    <t>UC08 - Receber Pagamento</t>
+  </si>
+  <si>
+    <t>Retirada do dinheiro referente às vendas ???</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <bgColor rgb="FFFFFFFF"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -204,234 +234,554 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
-      <alignment vertical="bottom" horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+  <a:themeElements>
+    <a:clrScheme name="Escritório">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Escritório">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Escritório">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="2" customWidth="1" max="2" width="54.0"/>
-    <col min="3" customWidth="1" max="3" width="29.14"/>
-    <col min="5" customWidth="1" max="5" width="24.29"/>
+    <col min="2" max="2" width="54" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c t="s" r="A2">
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="B2">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="C2">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3">
-      <c t="s" r="A3">
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="B3">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c t="s" r="C3">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4">
-      <c t="s" r="A4">
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c t="s" r="B4">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c t="s" r="C4">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5">
-      <c t="s" r="A5">
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c t="s" r="B5">
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c t="s" r="C5">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6">
-      <c t="s" r="A6">
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="B6">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c t="s" r="C6">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7">
-      <c t="s" r="A7">
+    <row r="7" spans="1:5" ht="51">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c t="s" r="B7">
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c t="s" r="C7">
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8">
-      <c t="s" r="A8">
+      <c r="D7" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c t="s" r="B8">
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c t="s" r="C8">
+      <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c t="s" r="E8">
+      <c r="E8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9">
-      <c t="s" r="A9">
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c t="s" r="B9">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c t="s" r="C9">
+      <c r="C9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10">
-      <c t="s" r="A10">
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c t="s" r="B10">
+      <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c t="s" r="C10">
+      <c r="C10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11">
-      <c t="s" r="A11">
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c t="s" r="B11">
+      <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c t="s" r="C11">
+      <c r="C11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12">
-      <c t="s" r="A12">
+      <c r="D11" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="25.5">
+      <c r="A12" t="s">
         <v>34</v>
       </c>
-      <c t="s" r="B12">
+      <c r="B12" t="s">
         <v>35</v>
       </c>
-      <c t="s" r="C12">
+      <c r="C12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13">
-      <c t="s" s="1" r="E13">
+      <c r="D12" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="B13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14">
-      <c t="s" r="E14">
+    <row r="14" spans="1:5">
+      <c r="B14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15">
-      <c t="s" r="E15">
+    <row r="15" spans="1:5">
+      <c r="B15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16">
-      <c t="s" r="E16">
+    <row r="16" spans="1:5">
+      <c r="D16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17">
-      <c t="s" r="E17">
+    <row r="17" spans="4:4">
+      <c r="D17" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18">
-      <c t="s" r="E18">
+    <row r="18" spans="4:4">
+      <c r="D18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19">
-      <c t="s" r="E19">
+    <row r="19" spans="4:4">
+      <c r="D19" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20">
-      <c t="s" r="E20">
+    <row r="20" spans="4:4">
+      <c r="D20" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21">
-      <c t="s" r="E21">
+    <row r="21" spans="4:4">
+      <c r="D21" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22">
-      <c t="s" r="E22">
+    <row r="22" spans="4:4">
+      <c r="D22" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23">
-      <c t="s" r="E23">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24">
-      <c t="s" r="E24">
+    <row r="23" spans="4:4">
+      <c r="D23" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25">
-      <c t="s" r="E25">
+    <row r="24" spans="4:4">
+      <c r="D24" s="2" t="s">
         <v>49</v>
       </c>
     </row>
+    <row r="25" spans="4:4">
+      <c r="D25" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" ht="12.75" customHeight="1">
+      <c r="D26" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização da 3ª Entrega
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
   <si>
     <t>REQ(01)</t>
   </si>
@@ -154,6 +154,30 @@
   </si>
   <si>
     <t>UC09 - Carregar Troco</t>
+  </si>
+  <si>
+    <t>UC10 - Recolher Numerário</t>
+  </si>
+  <si>
+    <t>UC11 - Emitir Ingresso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REQ(13) </t>
+  </si>
+  <si>
+    <t>Após todo o processo feito com sucesso, o cliente recebeo ticket para assistir o filme (Cliente)</t>
+  </si>
+  <si>
+    <t>Emitir Ingresso</t>
+  </si>
+  <si>
+    <t>REQ(14)</t>
+  </si>
+  <si>
+    <t>Após várias vendas acumuladas, o responsável pela máquina e pelo sistema, vai até as máquinas retirar as quantias (Gerente)</t>
+  </si>
+  <si>
+    <t>Recolher Numerário</t>
   </si>
 </sst>
 </file>
@@ -474,13 +498,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="103.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="108.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.140625" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" customWidth="1"/>
   </cols>
@@ -621,11 +647,29 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
       <c r="E14" t="s">
         <v>36</v>
       </c>
@@ -668,6 +712,16 @@
     <row r="22" spans="5:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E22" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>